<commit_message>
Completed the pipeline just need to tune the model
</commit_message>
<xml_diff>
--- a/MLB/todays_data.xlsx
+++ b/MLB/todays_data.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbkaplinger/Desktop/Random-Projects/MLB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47C5E62-5DBB-574D-9980-4911574AC7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B79099D-3124-CA40-A5CA-0F3A9753C932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="5-10-24" sheetId="1" r:id="rId1"/>
+    <sheet name="6-6-24" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Games</t>
   </si>
@@ -28,64 +28,34 @@
     <t>RFPred</t>
   </si>
   <si>
-    <t>('LAD', 'SD')</t>
+    <t>('CLE', 'KC')</t>
   </si>
   <si>
     <t>('OAK', 'SEA')</t>
   </si>
   <si>
-    <t>('MIL', 'STL')</t>
-  </si>
-  <si>
-    <t>('MIA', 'PHI')</t>
-  </si>
-  <si>
-    <t>('CHC', 'PIT')</t>
-  </si>
-  <si>
-    <t>('DET', 'HOU')</t>
-  </si>
-  <si>
-    <t>('CLE', 'CWS')</t>
-  </si>
-  <si>
-    <t>('CIN', 'SF')</t>
-  </si>
-  <si>
-    <t>('ATL', 'NYM')</t>
-  </si>
-  <si>
-    <t>('KC', 'LAA')</t>
-  </si>
-  <si>
-    <t>('NYY', 'TB')</t>
-  </si>
-  <si>
-    <t>('MIN', 'TOR')</t>
-  </si>
-  <si>
-    <t>('COL', 'TEX')</t>
-  </si>
-  <si>
-    <t>('ARI', 'BAL')</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Percent</t>
-  </si>
-  <si>
-    <t>NRFI</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
+    <t>('COL', 'STL')</t>
+  </si>
+  <si>
+    <t>('BOS', 'CWS')</t>
+  </si>
+  <si>
+    <t>('ATL', 'WSH')</t>
+  </si>
+  <si>
+    <t>('MIN', 'NYY')</t>
+  </si>
+  <si>
+    <t>('CHC', 'CIN')</t>
+  </si>
+  <si>
+    <t>('BAL', 'TOR')</t>
+  </si>
+  <si>
+    <t>('AZ', 'SD')</t>
+  </si>
+  <si>
+    <t>('LAD', 'PIT')</t>
   </si>
 </sst>
 </file>
@@ -104,7 +74,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -449,214 +418,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>2.8925797887850791E-3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>3.1837094127158379E-3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>4.6430673322659039E-3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.93300000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>6.3931657458652803E-3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>7.3005598012430301E-3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.89900000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>9.6259081298112163E-3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.77900000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>9.899774386864884E-3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.72899999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>1.0837635542662E-2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.61299999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>1.13232987775999E-2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.32400000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
-        <v>2.2012446970665629E-2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>2.299535816704662E-2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>2.687365860376981E-2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>3.7087499367576202E-2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>0.18443321330524259</v>
-      </c>
-      <c r="C15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
+        <v>0.22900000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Gradient Boosting and tuned the models
</commit_message>
<xml_diff>
--- a/MLB/todays_data.xlsx
+++ b/MLB/todays_data.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbkaplinger/Desktop/Random-Projects/MLB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B79099D-3124-CA40-A5CA-0F3A9753C932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A050CD41-7FDA-3E44-8794-44A4AC3DCC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="6-6-24" sheetId="1" r:id="rId1"/>
+    <sheet name="6-8-24" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Games</t>
   </si>
@@ -28,34 +28,61 @@
     <t>RFPred</t>
   </si>
   <si>
-    <t>('CLE', 'KC')</t>
-  </si>
-  <si>
-    <t>('OAK', 'SEA')</t>
+    <t>('KC', 'SEA')</t>
+  </si>
+  <si>
+    <t>('MIN', 'PIT')</t>
+  </si>
+  <si>
+    <t>('LAD', 'NYY')</t>
+  </si>
+  <si>
+    <t>('NYM', 'PHI')</t>
+  </si>
+  <si>
+    <t>('DET', 'MIL')</t>
+  </si>
+  <si>
+    <t>('SF', 'TEX')</t>
+  </si>
+  <si>
+    <t>('BAL', 'TB')</t>
+  </si>
+  <si>
+    <t>('ATL', 'WSH')</t>
+  </si>
+  <si>
+    <t>('BOS', 'CWS')</t>
+  </si>
+  <si>
+    <t>('CHC', 'CIN')</t>
+  </si>
+  <si>
+    <t>('AZ', 'SD')</t>
+  </si>
+  <si>
+    <t>('HOU', 'LAA')</t>
+  </si>
+  <si>
+    <t>('OAK', 'TOR')</t>
   </si>
   <si>
     <t>('COL', 'STL')</t>
   </si>
   <si>
-    <t>('BOS', 'CWS')</t>
-  </si>
-  <si>
-    <t>('ATL', 'WSH')</t>
-  </si>
-  <si>
-    <t>('MIN', 'NYY')</t>
-  </si>
-  <si>
-    <t>('CHC', 'CIN')</t>
-  </si>
-  <si>
-    <t>('BAL', 'TOR')</t>
-  </si>
-  <si>
-    <t>('AZ', 'SD')</t>
-  </si>
-  <si>
-    <t>('LAD', 'PIT')</t>
+    <t>('CLE', 'MIA')</t>
+  </si>
+  <si>
+    <t>NRFI</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Percent</t>
   </si>
 </sst>
 </file>
@@ -74,6 +101,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -418,100 +446,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.93600000000000005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.93600000000000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0.83399999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.93300000000000005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0.79200000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0.78600000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.89900000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0.77500000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.77900000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0.72399999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.72899999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0.67500000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.61299999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0.55500000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.32400000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0.54500000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.22900000000000001</v>
+        <v>0.51300000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>0.47699999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0.32800000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>4.9000000000000002E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added XGBoost model, tuned all of the models using CV, and got rid of SIERA as a feature
</commit_message>
<xml_diff>
--- a/MLB/todays_data.xlsx
+++ b/MLB/todays_data.xlsx
@@ -8,19 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbkaplinger/Desktop/Random-Projects/MLB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A050CD41-7FDA-3E44-8794-44A4AC3DCC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2BFE1B-4C67-9048-8499-2F3E9B8816E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="6-8-24" sheetId="1" r:id="rId1"/>
+    <sheet name="6-9-24" sheetId="2" r:id="rId2"/>
+    <sheet name="6-10-24" sheetId="3" r:id="rId3"/>
+    <sheet name="6-11-24" sheetId="4" r:id="rId4"/>
+    <sheet name="6-12-24" sheetId="5" r:id="rId5"/>
+    <sheet name="6-13-24" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="40">
   <si>
     <t>Games</t>
   </si>
@@ -28,6 +46,18 @@
     <t>RFPred</t>
   </si>
   <si>
+    <t>NRFI</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Percent</t>
+  </si>
+  <si>
     <t>('KC', 'SEA')</t>
   </si>
   <si>
@@ -73,29 +103,104 @@
     <t>('CLE', 'MIA')</t>
   </si>
   <si>
-    <t>NRFI</t>
-  </si>
-  <si>
-    <t>Correct</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Percent</t>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>('KC', 'NYY')</t>
+  </si>
+  <si>
+    <t>('CWS', 'SEA')</t>
+  </si>
+  <si>
+    <t>('OAK', 'SD')</t>
+  </si>
+  <si>
+    <t>('HOU', 'SF')</t>
+  </si>
+  <si>
+    <t>('COL', 'MIN')</t>
+  </si>
+  <si>
+    <t>('MIL', 'TOR')</t>
+  </si>
+  <si>
+    <t>('BOS', 'PHI')</t>
+  </si>
+  <si>
+    <t>('LAD', 'TEX')</t>
+  </si>
+  <si>
+    <t>('PIT', 'STL')</t>
+  </si>
+  <si>
+    <t>('AZ', 'LAA')</t>
+  </si>
+  <si>
+    <t>('CIN', 'CLE')</t>
+  </si>
+  <si>
+    <t>('ATL', 'BAL')</t>
+  </si>
+  <si>
+    <t>('DET', 'WSH')</t>
+  </si>
+  <si>
+    <t>('CHC', 'TB')</t>
+  </si>
+  <si>
+    <t>('MIA', 'NYM')</t>
+  </si>
+  <si>
+    <t>('MIN', 'OAK')</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -112,7 +217,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -135,13 +240,103 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -446,15 +641,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,136 +657,1073 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>0.93400000000000005</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>COUNTIF(D:D, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <f>COUNTA(D2:D20)</f>
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <f>E2/F2*100</f>
+        <v>42.857142857142854</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>0.83399999999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0.79200000000000004</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>0.78600000000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>0.77500000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>0.72399999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>0.67500000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>0.55500000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>0.54500000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>0.51300000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>0.47699999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>0.32800000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2">
+        <f>COUNTIF(D:D, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>COUNTA(D2:D20)</f>
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <f>E2/F2*100</f>
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>0.64900000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>0.64500000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>0.56699999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.48399999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.56100000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>0.47699999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.50700000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B14">
-        <v>0.32800000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.38100000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B15">
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.28299999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B16">
-        <v>4.9000000000000002E-2</v>
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>COUNTIF(D:D, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>COUNTA(D2:D20)</f>
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <f>E2/F2*100</f>
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>0.65800000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>0.47199999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7">
+        <v>0.46700000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2">
+        <f>COUNTIF(D:D, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>COUNTA(D2:D20)</f>
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <f>E2/F2*100</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>0.92</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>0.755</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>0.66700000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8">
+        <v>0.66300000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>0.63300000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10">
+        <v>0.59199999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11">
+        <v>0.56699999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <v>0.56399999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13">
+        <v>0.55500000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <v>0.52300000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15">
+        <v>0.51700000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>0.33400000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>0.99</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2">
+        <f>COUNTIF(D:D, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <f>COUNTA(D2:D20)</f>
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <f>E2/F2*100</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <v>0.753</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8">
+        <v>0.69399999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9">
+        <v>0.52600000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10">
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14">
+        <v>0.46300000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16">
+        <v>0.182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>COUNTIF(D:D, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>COUNTA(D2:D20)</f>
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <f>E2/F2*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>0.68200000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>0.67800000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>0.64500000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>0.627</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>0.54100000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10">
+        <v>0.40500000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11">
+        <v>0.30199999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added markdown to the notebook
</commit_message>
<xml_diff>
--- a/MLB/todays_data.xlsx
+++ b/MLB/todays_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbkaplinger/Desktop/Random-Projects/MLB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2BFE1B-4C67-9048-8499-2F3E9B8816E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FBF10A-28B0-A145-94FC-53B066A6372A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="6-8-24" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="6-11-24" sheetId="4" r:id="rId4"/>
     <sheet name="6-12-24" sheetId="5" r:id="rId5"/>
     <sheet name="6-13-24" sheetId="6" r:id="rId6"/>
+    <sheet name="6-14-24" sheetId="7" r:id="rId7"/>
+    <sheet name="06-15-24" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="54">
   <si>
     <t>Games</t>
   </si>
@@ -157,20 +159,74 @@
     <t>('MIN', 'OAK')</t>
   </si>
   <si>
+    <t>('MIA', 'WSH')</t>
+  </si>
+  <si>
+    <t>('AZ', 'CWS')</t>
+  </si>
+  <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>('KC', 'LAD')</t>
+  </si>
+  <si>
+    <t>('CIN', 'MIL')</t>
+  </si>
+  <si>
+    <t>('SEA', 'TEX')</t>
+  </si>
+  <si>
+    <t>('BAL', 'PHI')</t>
+  </si>
+  <si>
+    <t>('LAA', 'SF')</t>
+  </si>
+  <si>
+    <t>('ATL', 'TB')</t>
+  </si>
+  <si>
+    <t>('BOS', 'NYY')</t>
+  </si>
+  <si>
+    <t>('CLE', 'TOR')</t>
+  </si>
+  <si>
+    <t>('NYM', 'SD')</t>
+  </si>
+  <si>
+    <t>('DET', 'HOU')</t>
+  </si>
+  <si>
+    <t>('CHC', 'STL')</t>
+  </si>
+  <si>
+    <t>('COL', 'PIT')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -217,7 +273,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -315,11 +371,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -337,6 +423,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1582,8 +1674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1626,7 +1718,7 @@
       </c>
       <c r="E2">
         <f>COUNTIF(D:D, 1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <f>COUNTA(D2:D20)</f>
@@ -1634,7 +1726,7 @@
       </c>
       <c r="H2">
         <f>E2/F2*100</f>
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1644,11 +1736,11 @@
       <c r="B3">
         <v>0.84699999999999998</v>
       </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s">
-        <v>39</v>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1724,6 +1816,391 @@
       </c>
       <c r="C12" t="s">
         <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2">
+        <f>COUNTIF(D:D, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <f>COUNTA(D2:D20)</f>
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <f>E2/F2*100</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4">
+        <v>0.9</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5">
+        <v>0.83</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8">
+        <v>0.69599999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9">
+        <v>0.64400000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10">
+        <v>0.60499999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11">
+        <v>0.52500000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12">
+        <v>0.51400000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>0.49299999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14">
+        <v>0.45500000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15">
+        <v>0.45200000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16">
+        <v>0.44800000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2">
+        <f>COUNTIF(D:D, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>COUNTA(D2:D20)</f>
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <f>E2/F2*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7">
+        <v>0.69399999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8">
+        <v>0.61399999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>0.59299999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10">
+        <v>0.47099999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11">
+        <v>0.45100000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12">
+        <v>0.439</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13">
+        <v>0.40300000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16">
+        <v>0.222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Retuned the NRFI models after adding rolling averages
</commit_message>
<xml_diff>
--- a/MLB/todays_data.xlsx
+++ b/MLB/todays_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbkaplinger/Desktop/Random-Projects/MLB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8DCE1F-1284-FD4A-B988-0DC4DF0AC1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FD2DB8-C5BC-CE43-91F0-C4C11F2F6632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" firstSheet="2" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="2" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="6-8-24" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="93">
   <si>
     <t>Games</t>
   </si>
@@ -322,16 +322,13 @@
     <t>('KC', 'MIA')</t>
   </si>
   <si>
+    <t>('AZ', 'MIN')</t>
+  </si>
+  <si>
+    <t>('COL', 'HOU')</t>
+  </si>
+  <si>
     <t>('NYM', 'NYY')</t>
-  </si>
-  <si>
-    <t>('AZ', 'MIN')</t>
-  </si>
-  <si>
-    <t>('COL', 'HOU')</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -2643,7 +2640,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2828,7 +2825,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2858,104 +2855,119 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="B2">
-        <v>0.98</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2">
         <f>COUNTIF(D:D, 1)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F2">
         <f>COUNTA(D2:D20)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H2">
         <f>E2/F2*100</f>
-        <v>0</v>
+        <v>42.857142857142854</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="B3">
-        <v>0.94</v>
-      </c>
-      <c r="D3" t="s">
-        <v>93</v>
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B4">
-        <v>0.92900000000000005</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="B5">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="B6">
-        <v>0.86799999999999999</v>
-      </c>
-      <c r="D6" t="s">
-        <v>93</v>
+        <v>0.81</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B7">
-        <v>0.84099999999999997</v>
-      </c>
-      <c r="D7" t="s">
-        <v>93</v>
+        <v>0.748</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B8">
-        <v>0.76700000000000002</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B9">
-        <v>0.66600000000000004</v>
+        <v>0.63800000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B10">
-        <v>0.64800000000000002</v>
+        <v>0.60799999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -2963,7 +2975,7 @@
         <v>84</v>
       </c>
       <c r="B11">
-        <v>0.58699999999999997</v>
+        <v>0.58299999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -2971,31 +2983,37 @@
         <v>81</v>
       </c>
       <c r="B12">
-        <v>0.55400000000000005</v>
+        <v>0.53700000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="B13">
-        <v>0.55200000000000005</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="B14">
-        <v>0.47299999999999998</v>
+        <v>0.41199999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B15">
-        <v>0.40100000000000002</v>
+        <v>0.222</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -3003,10 +3021,13 @@
         <v>92</v>
       </c>
       <c r="B16">
-        <v>0.21199999999999999</v>
-      </c>
-      <c r="D16" t="s">
-        <v>93</v>
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete revamp, rolling averages of NRFI, wOBA, xwOBA
</commit_message>
<xml_diff>
--- a/MLB/todays_data.xlsx
+++ b/MLB/todays_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbkaplinger/Desktop/Random-Projects/MLB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FD2DB8-C5BC-CE43-91F0-C4C11F2F6632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF9B06D-E1E7-EF41-B0CC-3AA4851225C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="2" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" firstSheet="6" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="6-8-24" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,8 @@
     <sheet name="06-23-24" sheetId="16" r:id="rId16"/>
     <sheet name="06-24-24" sheetId="17" r:id="rId17"/>
     <sheet name="06-25-24" sheetId="18" r:id="rId18"/>
+    <sheet name="06-26-24" sheetId="19" r:id="rId19"/>
+    <sheet name="06-27-24" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="101">
   <si>
     <t>Games</t>
   </si>
@@ -329,19 +331,55 @@
   </si>
   <si>
     <t>('NYM', 'NYY')</t>
+  </si>
+  <si>
+    <t>('CLE', 'KC')</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>('DET', 'LAA')</t>
+  </si>
+  <si>
+    <t>('BAL', 'TEX')</t>
+  </si>
+  <si>
+    <t>('NYY', 'TOR')</t>
+  </si>
+  <si>
+    <t>('MIA', 'PHI')</t>
+  </si>
+  <si>
+    <t>('CIN', 'STL')</t>
+  </si>
+  <si>
+    <t>('ATL', 'CWS')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -460,7 +498,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -738,11 +776,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -796,6 +864,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2824,8 +2898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3028,6 +3102,203 @@
       </c>
       <c r="D16">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>COUNTIF(D:D, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>COUNTA(D2:D20)</f>
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <f>E2/F2*100</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5">
+        <v>0.73399999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6">
+        <v>0.73099999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7">
+        <v>0.72599999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8">
+        <v>0.66100000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9">
+        <v>0.66100000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10">
+        <v>0.63800000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11">
+        <v>0.54900000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12">
+        <v>0.499</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13">
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14">
+        <v>0.33600000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15">
+        <v>0.189</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3235,6 +3506,149 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2">
+        <v>1.0029999999999999</v>
+      </c>
+      <c r="D2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2">
+        <f>COUNTIF(D:D, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>COUNTA(D2:D20)</f>
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <f>E2/F2*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7">
+        <v>0.58599999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8">
+        <v>0.54700000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9">
+        <v>0.45900000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10">
+        <v>0.40200000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H8"/>

</xml_diff>